<commit_message>
adding new graph module
</commit_message>
<xml_diff>
--- a/data/quarterly_reports/FB_quarterly_report.xlsx
+++ b/data/quarterly_reports/FB_quarterly_report.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bykov\Jupyter notebooks\Dastocks\data\quarterly_reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF372237-2563-4ED2-B92A-FD8C5DDA1120}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -445,8 +451,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,17 +511,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -553,9 +567,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,9 +601,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -621,9 +653,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -796,14 +846,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -832,7 +891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -861,7 +920,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -890,7 +949,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -919,7 +978,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -948,7 +1007,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -977,7 +1036,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -997,7 +1056,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1026,7 +1085,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1055,7 +1114,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1084,7 +1143,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1113,7 +1172,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1142,7 +1201,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1171,7 +1230,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1200,7 +1259,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1229,7 +1288,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1258,7 +1317,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1287,7 +1346,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1316,7 +1375,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>